<commit_message>
edited data to be used in AGB analysis
</commit_message>
<xml_diff>
--- a/Data/AGB_intens.xlsx
+++ b/Data/AGB_intens.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="76">
   <si>
     <t>Site</t>
   </si>
@@ -121,24 +121,12 @@
     <t>Bryan et al 2010b</t>
   </si>
   <si>
-    <t>Chambers et al 2005a</t>
-  </si>
-  <si>
-    <t>Chambers et al 2005</t>
-  </si>
-  <si>
     <t>SD</t>
   </si>
   <si>
     <t>Americas</t>
   </si>
   <si>
-    <t>Chambers et al 2005b</t>
-  </si>
-  <si>
-    <t>Chambers et al 2005c</t>
-  </si>
-  <si>
     <t>d'Oliveira et al 2012a</t>
   </si>
   <si>
@@ -166,39 +154,6 @@
     <t>Imai et al 2013</t>
   </si>
   <si>
-    <t>Imai et al 2013b</t>
-  </si>
-  <si>
-    <t>Kronseder et al 2012a</t>
-  </si>
-  <si>
-    <t>Kronseder et al 2012</t>
-  </si>
-  <si>
-    <t>Kronseder et al 2012b</t>
-  </si>
-  <si>
-    <t>Lasco et al 2006a</t>
-  </si>
-  <si>
-    <t>Lasco et al 2006</t>
-  </si>
-  <si>
-    <t>Lasco et al 2006b</t>
-  </si>
-  <si>
-    <t>Lasco et al 2006c</t>
-  </si>
-  <si>
-    <t>Lasco et al 2006d</t>
-  </si>
-  <si>
-    <t>Lasco et al 2006e</t>
-  </si>
-  <si>
-    <t>Lindner et al 2011</t>
-  </si>
-  <si>
     <t>Mazzei et al 2010</t>
   </si>
   <si>
@@ -269,12 +224,6 @@
   </si>
   <si>
     <t>Sist et al 2012b</t>
-  </si>
-  <si>
-    <t>Sist et al 2014a</t>
-  </si>
-  <si>
-    <t>Sist et al 2014</t>
   </si>
   <si>
     <t>Tangki et al 2008</t>
@@ -1121,16 +1070,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="V43" sqref="V43"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X33" sqref="X33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="21" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
@@ -1198,13 +1147,13 @@
         <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="W1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="X1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
@@ -1278,7 +1227,7 @@
         <v>22</v>
       </c>
       <c r="X2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -1352,7 +1301,7 @@
         <v>22</v>
       </c>
       <c r="X3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
@@ -1423,10 +1372,10 @@
         <v>50</v>
       </c>
       <c r="W4" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="X4" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
@@ -1497,60 +1446,60 @@
         <v>50</v>
       </c>
       <c r="W5" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="X5" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>6.9</v>
+      </c>
+      <c r="G6">
+        <v>198.9</v>
+      </c>
+      <c r="H6">
+        <v>8.5</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>185.1</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
         <v>36</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6">
-        <v>-9999</v>
-      </c>
-      <c r="G6">
-        <v>346.8</v>
-      </c>
-      <c r="H6">
-        <v>28.213294739999998</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>279.93333330000002</v>
-      </c>
-      <c r="K6">
-        <v>29.850348969999999</v>
-      </c>
-      <c r="L6">
-        <v>3</v>
-      </c>
-      <c r="M6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6">
-        <v>8</v>
-      </c>
-      <c r="O6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" t="s">
-        <v>38</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -1558,14 +1507,23 @@
       <c r="R6">
         <v>1</v>
       </c>
-      <c r="S6" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" t="s">
-        <v>22</v>
+      <c r="S6">
+        <v>6.9</v>
+      </c>
+      <c r="T6">
+        <v>1.8665815649999999</v>
       </c>
       <c r="U6" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="V6">
+        <v>35</v>
+      </c>
+      <c r="W6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -1573,425 +1531,443 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
+      <c r="E7">
+        <v>5.7</v>
       </c>
       <c r="F7">
-        <v>-9999</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="G7">
-        <v>330.83333329999999</v>
+        <v>258</v>
       </c>
       <c r="H7">
-        <v>30.918656720000001</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
       <c r="J7">
-        <v>261.39999999999998</v>
+        <v>198</v>
       </c>
       <c r="K7">
-        <v>28.729253379999999</v>
+        <v>18</v>
       </c>
       <c r="L7">
         <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q7">
         <v>1</v>
       </c>
       <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T7" t="s">
-        <v>22</v>
+        <v>0.5</v>
+      </c>
+      <c r="S7">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="T7">
+        <v>5.7</v>
       </c>
       <c r="U7" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="V7" t="s">
+        <v>22</v>
+      </c>
+      <c r="W7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
       <c r="C8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
+      <c r="E8">
+        <v>10</v>
       </c>
       <c r="F8">
-        <v>-9999</v>
+        <v>69</v>
       </c>
       <c r="G8">
-        <v>343.3</v>
+        <v>258</v>
       </c>
       <c r="H8">
-        <v>32.22002483</v>
+        <v>30</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8">
-        <v>249.7333333</v>
+        <v>148</v>
       </c>
       <c r="K8">
-        <v>15.297494349999999</v>
+        <v>10</v>
       </c>
       <c r="L8">
         <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N8">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q8">
         <v>1</v>
       </c>
       <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8" t="s">
-        <v>22</v>
-      </c>
-      <c r="T8" t="s">
-        <v>22</v>
+        <v>0.5</v>
+      </c>
+      <c r="S8">
+        <v>69</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
       </c>
       <c r="U8" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="V8" t="s">
+        <v>22</v>
+      </c>
+      <c r="W8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
-        <v>22</v>
+      <c r="E9">
+        <v>5.5</v>
       </c>
       <c r="F9">
-        <v>6.9</v>
+        <v>66</v>
       </c>
       <c r="G9">
-        <v>198.9</v>
+        <v>386.42533329999998</v>
       </c>
       <c r="H9">
-        <v>8.5</v>
+        <v>68.073639389999997</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J9">
-        <v>185.1</v>
+        <v>284.77433330000002</v>
       </c>
       <c r="K9">
-        <v>9</v>
+        <v>36.796639740000003</v>
       </c>
       <c r="L9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N9">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="O9" t="s">
         <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="Q9">
         <v>1</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S9">
-        <v>6.9</v>
+        <v>66</v>
       </c>
       <c r="T9">
-        <v>1.8665815649999999</v>
+        <v>5.5</v>
       </c>
       <c r="U9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="V9">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="W9" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="X9" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E10">
-        <v>5.7</v>
+        <v>2.36</v>
       </c>
       <c r="F10">
-        <v>35.299999999999997</v>
+        <v>13.74</v>
       </c>
       <c r="G10">
-        <v>258</v>
+        <v>499</v>
       </c>
       <c r="H10">
+        <v>60</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>341</v>
+      </c>
+      <c r="K10">
+        <v>52</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10">
         <v>30</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <v>198</v>
-      </c>
-      <c r="K10">
-        <v>18</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-      <c r="M10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10">
-        <v>12</v>
       </c>
       <c r="O10" t="s">
         <v>24</v>
       </c>
       <c r="P10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="Q10">
         <v>1</v>
       </c>
-      <c r="R10">
-        <v>0.5</v>
+      <c r="R10" t="s">
+        <v>22</v>
       </c>
       <c r="S10">
-        <v>35.299999999999997</v>
+        <v>13.74</v>
       </c>
       <c r="T10">
-        <v>5.7</v>
+        <v>2.36</v>
       </c>
       <c r="U10" t="s">
-        <v>38</v>
-      </c>
-      <c r="V10" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="V10">
+        <v>60</v>
       </c>
       <c r="W10" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="X10" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>8.4</v>
       </c>
       <c r="F11">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="G11">
-        <v>258</v>
+        <v>409.8</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="J11">
-        <v>148</v>
+        <v>315.36470589999999</v>
       </c>
       <c r="K11">
-        <v>10</v>
+        <v>44.909073990000003</v>
       </c>
       <c r="L11">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N11">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O11" t="s">
         <v>24</v>
       </c>
       <c r="P11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q11">
         <v>1</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="T11">
-        <v>10</v>
+        <v>8.4</v>
       </c>
       <c r="U11" t="s">
-        <v>38</v>
-      </c>
-      <c r="V11" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="V11">
+        <v>55</v>
       </c>
       <c r="W11" t="s">
         <v>22</v>
       </c>
       <c r="X11" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E12">
-        <v>5.5</v>
+        <v>0.82</v>
       </c>
       <c r="F12">
-        <v>66</v>
+        <v>8.11</v>
       </c>
       <c r="G12">
-        <v>386.42533329999998</v>
+        <v>420.4</v>
       </c>
       <c r="H12">
-        <v>68.073639389999997</v>
+        <v>92.95</v>
       </c>
       <c r="I12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J12">
-        <v>284.77433330000002</v>
+        <v>386.22</v>
       </c>
       <c r="K12">
-        <v>36.796639740000003</v>
+        <v>109.0794186</v>
       </c>
       <c r="L12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N12">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O12" t="s">
         <v>24</v>
       </c>
       <c r="P12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Q12">
         <v>1</v>
       </c>
       <c r="R12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>66</v>
+        <v>8.11</v>
       </c>
       <c r="T12">
-        <v>5.5</v>
+        <v>0.82</v>
       </c>
       <c r="U12" t="s">
         <v>26</v>
       </c>
-      <c r="V12">
-        <v>80</v>
+      <c r="V12" t="s">
+        <v>22</v>
       </c>
       <c r="W12" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="X12" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -2001,133 +1977,133 @@
       <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13">
-        <v>8</v>
+      <c r="C13" t="s">
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
       </c>
       <c r="E13">
-        <v>2.36</v>
+        <v>0.39</v>
       </c>
       <c r="F13">
-        <v>13.74</v>
+        <v>5.66</v>
       </c>
       <c r="G13">
-        <v>499</v>
+        <v>380</v>
       </c>
       <c r="H13">
-        <v>60</v>
+        <v>86.78</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J13">
-        <v>341</v>
-      </c>
-      <c r="K13">
-        <v>52</v>
+        <v>353.02</v>
+      </c>
+      <c r="K13" t="s">
+        <v>22</v>
       </c>
       <c r="L13">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="M13" t="s">
         <v>23</v>
       </c>
       <c r="N13">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O13" t="s">
         <v>24</v>
       </c>
       <c r="P13" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="Q13">
         <v>1</v>
       </c>
-      <c r="R13" t="s">
-        <v>22</v>
+      <c r="R13">
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>13.74</v>
+        <v>5.7</v>
       </c>
       <c r="T13">
-        <v>2.36</v>
+        <v>0.39</v>
       </c>
       <c r="U13" t="s">
         <v>26</v>
       </c>
-      <c r="V13">
-        <v>60</v>
+      <c r="V13" t="s">
+        <v>22</v>
       </c>
       <c r="W13" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="X13" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14">
-        <v>5</v>
+      <c r="C14" t="s">
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>0.39</v>
       </c>
       <c r="F14">
-        <v>-9999</v>
+        <v>5.66</v>
       </c>
       <c r="G14">
-        <v>499</v>
+        <v>380</v>
       </c>
       <c r="H14">
-        <v>60</v>
+        <v>86.78</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J14">
-        <v>163</v>
-      </c>
-      <c r="K14">
-        <v>84</v>
+        <v>353.02</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
       </c>
       <c r="L14">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="M14" t="s">
         <v>23</v>
       </c>
       <c r="N14">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O14" t="s">
         <v>24</v>
       </c>
       <c r="P14" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="Q14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>0.2</v>
-      </c>
-      <c r="S14" t="s">
-        <v>22</v>
-      </c>
-      <c r="T14" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>5.66</v>
+      </c>
+      <c r="T14">
+        <v>0.39</v>
       </c>
       <c r="U14" t="s">
         <v>26</v>
@@ -2139,148 +2115,166 @@
         <v>22</v>
       </c>
       <c r="X14" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
-        <v>22</v>
+      <c r="E15">
+        <v>0.76</v>
       </c>
       <c r="F15">
-        <v>-9999</v>
+        <v>11.38</v>
       </c>
       <c r="G15">
-        <v>228.1</v>
+        <v>387.3</v>
       </c>
       <c r="H15">
-        <v>98.1</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="I15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J15">
-        <v>159.9</v>
-      </c>
-      <c r="K15">
-        <v>88.2</v>
+        <v>335.40179999999998</v>
+      </c>
+      <c r="K15" t="s">
+        <v>22</v>
       </c>
       <c r="L15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="M15" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N15">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="O15" t="s">
         <v>24</v>
       </c>
       <c r="P15" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="Q15">
         <v>1</v>
       </c>
       <c r="R15">
-        <v>0.06</v>
-      </c>
-      <c r="S15" t="s">
-        <v>22</v>
-      </c>
-      <c r="T15" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>11.4</v>
+      </c>
+      <c r="T15">
+        <v>0.76</v>
       </c>
       <c r="U15" t="s">
         <v>26</v>
+      </c>
+      <c r="V15" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" t="s">
+        <v>22</v>
+      </c>
+      <c r="X15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
-        <v>22</v>
+      <c r="E16">
+        <v>0.76</v>
       </c>
       <c r="F16">
-        <v>-9999</v>
+        <v>11.38</v>
       </c>
       <c r="G16">
-        <v>547.1</v>
+        <v>387.3</v>
       </c>
       <c r="H16">
-        <v>193.8</v>
+        <v>81.010000000000005</v>
       </c>
       <c r="I16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J16">
-        <v>230.8</v>
-      </c>
-      <c r="K16">
-        <v>104.2</v>
+        <v>335.40179999999998</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
       </c>
       <c r="L16">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M16" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N16">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="O16" t="s">
         <v>24</v>
       </c>
       <c r="P16" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="Q16">
         <v>1</v>
       </c>
       <c r="R16">
-        <v>0.06</v>
-      </c>
-      <c r="S16" t="s">
-        <v>22</v>
-      </c>
-      <c r="T16" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>11.38</v>
+      </c>
+      <c r="T16">
+        <v>0.76</v>
       </c>
       <c r="U16" t="s">
         <v>26</v>
+      </c>
+      <c r="V16" t="s">
+        <v>22</v>
+      </c>
+      <c r="W16" t="s">
+        <v>22</v>
+      </c>
+      <c r="X16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17">
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
@@ -2289,31 +2283,31 @@
         <v>22</v>
       </c>
       <c r="F17">
-        <v>-9999</v>
+        <v>179</v>
       </c>
       <c r="G17">
-        <v>399</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H17">
-        <v>145</v>
+        <v>328.677753</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J17">
-        <v>191</v>
+        <v>127.1630665</v>
       </c>
       <c r="K17">
-        <v>123</v>
+        <v>75.411510320000005</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N17">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O17" t="s">
         <v>33</v>
@@ -2322,30 +2316,39 @@
         <v>25</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>0.1</v>
-      </c>
-      <c r="S17" t="s">
-        <v>22</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="S17">
+        <v>179</v>
       </c>
       <c r="T17" t="s">
         <v>22</v>
       </c>
       <c r="U17" t="s">
         <v>26</v>
+      </c>
+      <c r="V17" t="s">
+        <v>22</v>
+      </c>
+      <c r="W17" t="s">
+        <v>22</v>
+      </c>
+      <c r="X17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -2354,31 +2357,31 @@
         <v>22</v>
       </c>
       <c r="F18">
-        <v>-9999</v>
+        <v>150</v>
       </c>
       <c r="G18">
-        <v>399</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H18">
-        <v>145</v>
+        <v>328.677753</v>
       </c>
       <c r="I18">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J18">
-        <v>238</v>
+        <v>92.938523090000004</v>
       </c>
       <c r="K18">
-        <v>156</v>
+        <v>44.10157135</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O18" t="s">
         <v>33</v>
@@ -2387,30 +2390,39 @@
         <v>25</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R18">
-        <v>0.1</v>
-      </c>
-      <c r="S18" t="s">
-        <v>22</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="S18">
+        <v>150</v>
       </c>
       <c r="T18" t="s">
         <v>22</v>
       </c>
       <c r="U18" t="s">
         <v>26</v>
+      </c>
+      <c r="V18" t="s">
+        <v>22</v>
+      </c>
+      <c r="W18" t="s">
+        <v>22</v>
+      </c>
+      <c r="X18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -2419,31 +2431,31 @@
         <v>22</v>
       </c>
       <c r="F19">
-        <v>-9999</v>
+        <v>150</v>
       </c>
       <c r="G19">
-        <v>399</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H19">
-        <v>145</v>
+        <v>328.677753</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J19">
-        <v>204</v>
+        <v>168.57521850000001</v>
       </c>
       <c r="K19">
-        <v>134</v>
+        <v>44.284300420000001</v>
       </c>
       <c r="L19">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N19">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O19" t="s">
         <v>33</v>
@@ -2452,30 +2464,39 @@
         <v>25</v>
       </c>
       <c r="Q19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19">
-        <v>0.1</v>
-      </c>
-      <c r="S19" t="s">
-        <v>22</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="S19">
+        <v>150</v>
       </c>
       <c r="T19" t="s">
         <v>22</v>
       </c>
       <c r="U19" t="s">
         <v>26</v>
+      </c>
+      <c r="V19" t="s">
+        <v>22</v>
+      </c>
+      <c r="W19" t="s">
+        <v>22</v>
+      </c>
+      <c r="X19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20">
-        <v>18.5</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -2484,31 +2505,31 @@
         <v>22</v>
       </c>
       <c r="F20">
-        <v>-9999</v>
+        <v>150</v>
       </c>
       <c r="G20">
-        <v>399</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H20">
-        <v>145</v>
+        <v>328.677753</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J20">
-        <v>235</v>
+        <v>168.59805729999999</v>
       </c>
       <c r="K20">
-        <v>161</v>
+        <v>116.5109326</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N20">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O20" t="s">
         <v>33</v>
@@ -2517,30 +2538,39 @@
         <v>25</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R20">
-        <v>0.1</v>
-      </c>
-      <c r="S20" t="s">
-        <v>22</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="S20">
+        <v>150</v>
       </c>
       <c r="T20" t="s">
         <v>22</v>
       </c>
       <c r="U20" t="s">
         <v>26</v>
+      </c>
+      <c r="V20" t="s">
+        <v>22</v>
+      </c>
+      <c r="W20" t="s">
+        <v>22</v>
+      </c>
+      <c r="X20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -2549,31 +2579,31 @@
         <v>22</v>
       </c>
       <c r="F21">
-        <v>-9999</v>
+        <v>179</v>
       </c>
       <c r="G21">
-        <v>399</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H21">
-        <v>145</v>
+        <v>328.677753</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J21">
-        <v>287</v>
+        <v>87.221436870000005</v>
       </c>
       <c r="K21">
-        <v>149</v>
+        <v>63.515759969999998</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="M21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N21">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O21" t="s">
         <v>33</v>
@@ -2582,30 +2612,39 @@
         <v>25</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R21">
-        <v>0.1</v>
-      </c>
-      <c r="S21" t="s">
-        <v>22</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="S21">
+        <v>179</v>
       </c>
       <c r="T21" t="s">
         <v>22</v>
       </c>
       <c r="U21" t="s">
         <v>26</v>
+      </c>
+      <c r="V21" t="s">
+        <v>22</v>
+      </c>
+      <c r="W21" t="s">
+        <v>22</v>
+      </c>
+      <c r="X21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C22">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
@@ -2614,188 +2653,197 @@
         <v>22</v>
       </c>
       <c r="F22">
-        <v>-9999</v>
+        <v>150</v>
       </c>
       <c r="G22">
-        <v>313</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H22">
-        <v>48</v>
+        <v>328.677753</v>
       </c>
       <c r="I22">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J22">
-        <v>204</v>
+        <v>181.832157</v>
       </c>
       <c r="K22">
-        <v>38</v>
+        <v>47.298146269999997</v>
       </c>
       <c r="L22">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O22" t="s">
         <v>33</v>
       </c>
       <c r="P22" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R22">
-        <v>0.05</v>
-      </c>
-      <c r="S22" t="s">
-        <v>22</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="S22">
+        <v>150</v>
       </c>
       <c r="T22" t="s">
         <v>22</v>
       </c>
       <c r="U22" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="V22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W22" t="s">
+        <v>22</v>
+      </c>
+      <c r="X22" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23">
-        <v>8.4</v>
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
       </c>
       <c r="F23">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="G23">
-        <v>409.8</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H23">
-        <v>64.900000000000006</v>
+        <v>328.677753</v>
       </c>
       <c r="I23">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J23">
-        <v>315.36470589999999</v>
+        <v>51.292534230000001</v>
       </c>
       <c r="K23">
-        <v>44.909073990000003</v>
+        <v>49.333246719999998</v>
       </c>
       <c r="L23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N23">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O23" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="P23" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R23">
-        <v>1</v>
+        <v>6.25E-2</v>
       </c>
       <c r="S23">
-        <v>21</v>
-      </c>
-      <c r="T23">
-        <v>8.4</v>
+        <v>179</v>
+      </c>
+      <c r="T23" t="s">
+        <v>22</v>
       </c>
       <c r="U23" t="s">
-        <v>38</v>
-      </c>
-      <c r="V23">
-        <v>55</v>
+        <v>26</v>
+      </c>
+      <c r="V23" t="s">
+        <v>22</v>
       </c>
       <c r="W23" t="s">
         <v>22</v>
       </c>
       <c r="X23" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24">
-        <v>0.82</v>
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
       </c>
       <c r="F24">
-        <v>8.11</v>
+        <v>179</v>
       </c>
       <c r="G24">
-        <v>420.4</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H24">
-        <v>92.95</v>
+        <v>328.677753</v>
       </c>
       <c r="I24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J24">
-        <v>386.22</v>
+        <v>67.347826119999993</v>
       </c>
       <c r="K24">
-        <v>109.0794186</v>
+        <v>69.933008979999997</v>
       </c>
       <c r="L24">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="M24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O24" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="P24" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="Q24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R24">
-        <v>1</v>
+        <v>6.25E-2</v>
       </c>
       <c r="S24">
-        <v>8.11</v>
-      </c>
-      <c r="T24">
-        <v>0.82</v>
+        <v>179</v>
+      </c>
+      <c r="T24" t="s">
+        <v>22</v>
       </c>
       <c r="U24" t="s">
         <v>26</v>
@@ -2807,352 +2855,388 @@
         <v>22</v>
       </c>
       <c r="X24" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25">
-        <v>0.39</v>
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
       </c>
       <c r="F25">
-        <v>5.66</v>
+        <v>179</v>
       </c>
       <c r="G25">
-        <v>380</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H25">
-        <v>86.78</v>
+        <v>328.677753</v>
       </c>
       <c r="I25">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J25">
-        <v>353.02</v>
-      </c>
-      <c r="K25" t="s">
-        <v>22</v>
+        <v>58.766026170000004</v>
+      </c>
+      <c r="K25">
+        <v>46.16436693</v>
       </c>
       <c r="L25">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N25">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="O25" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="P25" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>6.25E-2</v>
       </c>
       <c r="S25">
-        <v>5.7</v>
-      </c>
-      <c r="T25">
-        <v>0.39</v>
+        <v>179</v>
+      </c>
+      <c r="T25" t="s">
+        <v>22</v>
       </c>
       <c r="U25" t="s">
         <v>26</v>
+      </c>
+      <c r="V25" t="s">
+        <v>22</v>
+      </c>
+      <c r="W25" t="s">
+        <v>22</v>
+      </c>
+      <c r="X25" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26">
-        <v>0.39</v>
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
       </c>
       <c r="F26">
-        <v>5.66</v>
+        <v>179</v>
       </c>
       <c r="G26">
-        <v>380</v>
+        <v>565.10414960000003</v>
       </c>
       <c r="H26">
-        <v>86.78</v>
+        <v>328.677753</v>
       </c>
       <c r="I26">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J26">
-        <v>353.02</v>
-      </c>
-      <c r="K26" t="s">
-        <v>22</v>
+        <v>68.78087386</v>
+      </c>
+      <c r="K26">
+        <v>65.25066726</v>
       </c>
       <c r="L26">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M26" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N26">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="O26" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="P26" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R26">
-        <v>1</v>
+        <v>6.25E-2</v>
       </c>
       <c r="S26">
-        <v>5.66</v>
-      </c>
-      <c r="T26">
-        <v>0.39</v>
+        <v>179</v>
+      </c>
+      <c r="T26" t="s">
+        <v>22</v>
       </c>
       <c r="U26" t="s">
         <v>26</v>
+      </c>
+      <c r="V26" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" t="s">
+        <v>22</v>
+      </c>
+      <c r="X26" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" t="s">
-        <v>22</v>
+        <v>63</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
       </c>
-      <c r="E27">
-        <v>0.76</v>
+      <c r="E27" t="s">
+        <v>22</v>
       </c>
       <c r="F27">
-        <v>11.38</v>
+        <v>154.482125</v>
       </c>
       <c r="G27">
-        <v>387.3</v>
+        <v>333.47</v>
       </c>
       <c r="H27">
-        <v>81.010000000000005</v>
+        <v>40.73364703</v>
       </c>
       <c r="I27">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J27">
-        <v>335.40179999999998</v>
-      </c>
-      <c r="K27" t="s">
-        <v>22</v>
+        <v>135.80000000000001</v>
+      </c>
+      <c r="K27">
+        <v>20.751983039999999</v>
       </c>
       <c r="L27">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M27" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27">
         <v>23</v>
-      </c>
-      <c r="N27">
-        <v>32</v>
       </c>
       <c r="O27" t="s">
         <v>24</v>
       </c>
       <c r="P27" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="Q27">
         <v>1</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="S27">
-        <v>11.4</v>
-      </c>
-      <c r="T27">
-        <v>0.76</v>
+        <v>154.482125</v>
+      </c>
+      <c r="T27" t="s">
+        <v>22</v>
       </c>
       <c r="U27" t="s">
         <v>26</v>
+      </c>
+      <c r="V27" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" t="s">
+        <v>22</v>
+      </c>
+      <c r="X27" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
+        <v>63</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28">
-        <v>0.76</v>
+        <v>32</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
       </c>
       <c r="F28">
-        <v>11.38</v>
+        <v>103.5835</v>
       </c>
       <c r="G28">
-        <v>387.3</v>
+        <v>327.54000000000002</v>
       </c>
       <c r="H28">
-        <v>81.010000000000005</v>
+        <v>54.037106700000002</v>
       </c>
       <c r="I28">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J28">
-        <v>335.40179999999998</v>
-      </c>
-      <c r="K28" t="s">
-        <v>22</v>
+        <v>211.78</v>
+      </c>
+      <c r="K28">
+        <v>18.6400617</v>
       </c>
       <c r="L28">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M28" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="N28">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="O28" t="s">
         <v>24</v>
       </c>
       <c r="P28" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="Q28">
         <v>1</v>
       </c>
       <c r="R28">
-        <v>1</v>
+        <v>0.16</v>
       </c>
       <c r="S28">
-        <v>11.38</v>
+        <v>103.5835</v>
       </c>
       <c r="T28">
-        <v>0.76</v>
+        <v>24.059328000000001</v>
       </c>
       <c r="U28" t="s">
         <v>26</v>
+      </c>
+      <c r="V28">
+        <v>60</v>
+      </c>
+      <c r="W28" t="s">
+        <v>75</v>
+      </c>
+      <c r="X28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
         <v>10</v>
       </c>
-      <c r="D29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29">
-        <v>179</v>
-      </c>
       <c r="G29">
-        <v>565.10414960000003</v>
+        <v>113.9</v>
       </c>
       <c r="H29">
-        <v>328.677753</v>
+        <v>29.4</v>
       </c>
       <c r="I29">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J29">
-        <v>127.1630665</v>
+        <v>105.3</v>
       </c>
       <c r="K29">
-        <v>75.411510320000005</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="L29">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N29">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="O29" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P29" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>0.5</v>
+      </c>
+      <c r="S29">
+        <v>10</v>
+      </c>
+      <c r="T29">
         <v>2</v>
       </c>
-      <c r="R29">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S29">
-        <v>179</v>
-      </c>
-      <c r="T29" t="s">
-        <v>22</v>
-      </c>
       <c r="U29" t="s">
-        <v>26</v>
-      </c>
-      <c r="V29" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="V29">
+        <v>45</v>
       </c>
       <c r="W29" t="s">
         <v>22</v>
       </c>
       <c r="X29" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
@@ -3161,46 +3245,46 @@
         <v>22</v>
       </c>
       <c r="F30">
-        <v>150</v>
+        <v>117.38</v>
       </c>
       <c r="G30">
-        <v>565.10414960000003</v>
+        <v>256</v>
       </c>
       <c r="H30">
-        <v>328.677753</v>
+        <v>26.8</v>
       </c>
       <c r="I30">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J30">
-        <v>92.938523090000004</v>
+        <v>183.8</v>
       </c>
       <c r="K30">
-        <v>44.10157135</v>
+        <v>5.8</v>
       </c>
       <c r="L30">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N30">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O30" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P30" t="s">
         <v>25</v>
       </c>
       <c r="Q30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R30">
-        <v>6.25E-2</v>
+        <v>0.25</v>
       </c>
       <c r="S30">
-        <v>150</v>
+        <v>117.38</v>
       </c>
       <c r="T30" t="s">
         <v>22</v>
@@ -3208,1156 +3292,230 @@
       <c r="U30" t="s">
         <v>26</v>
       </c>
-      <c r="V30" t="s">
-        <v>22</v>
+      <c r="V30">
+        <v>60</v>
       </c>
       <c r="W30" t="s">
         <v>22</v>
       </c>
       <c r="X30" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
-      <c r="E31" t="s">
-        <v>22</v>
+      <c r="E31">
+        <v>21</v>
       </c>
       <c r="F31">
-        <v>150</v>
+        <v>-9999</v>
       </c>
       <c r="G31">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H31">
-        <v>328.677753</v>
+        <v>442.15679999999998</v>
+      </c>
+      <c r="H31" t="s">
+        <v>22</v>
       </c>
       <c r="I31">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J31">
-        <v>168.57521850000001</v>
-      </c>
-      <c r="K31">
-        <v>44.284300420000001</v>
+        <v>236.7577</v>
+      </c>
+      <c r="K31" t="s">
+        <v>22</v>
       </c>
       <c r="L31">
-        <v>9</v>
-      </c>
-      <c r="M31" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="N31">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="O31" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P31" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="Q31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R31">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S31">
-        <v>150</v>
-      </c>
-      <c r="T31" t="s">
-        <v>22</v>
+        <v>6.25</v>
+      </c>
+      <c r="S31" t="s">
+        <v>22</v>
+      </c>
+      <c r="T31">
+        <v>21</v>
       </c>
       <c r="U31" t="s">
-        <v>26</v>
-      </c>
-      <c r="V31" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="V31">
+        <v>55</v>
       </c>
       <c r="W31" t="s">
         <v>22</v>
       </c>
       <c r="X31" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32">
         <v>10</v>
       </c>
-      <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" t="s">
-        <v>22</v>
-      </c>
       <c r="F32">
-        <v>150</v>
+        <v>-9999</v>
       </c>
       <c r="G32">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H32">
-        <v>328.677753</v>
+        <v>406.6035</v>
+      </c>
+      <c r="H32" t="s">
+        <v>22</v>
       </c>
       <c r="I32">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J32">
-        <v>168.59805729999999</v>
-      </c>
-      <c r="K32">
-        <v>116.5109326</v>
+        <v>303.1123</v>
+      </c>
+      <c r="K32" t="s">
+        <v>22</v>
       </c>
       <c r="L32">
-        <v>8</v>
-      </c>
-      <c r="M32" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="N32">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="O32" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P32" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="Q32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R32">
-        <v>6.25E-2</v>
+        <v>6.25</v>
       </c>
       <c r="S32">
-        <v>150</v>
-      </c>
-      <c r="T32" t="s">
-        <v>22</v>
+        <v>38.826592419999997</v>
+      </c>
+      <c r="T32">
+        <v>10</v>
       </c>
       <c r="U32" t="s">
-        <v>26</v>
-      </c>
-      <c r="V32" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="V32">
+        <v>55</v>
       </c>
       <c r="W32" t="s">
         <v>22</v>
       </c>
       <c r="X32" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C33">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33">
+        <v>101.2</v>
+      </c>
+      <c r="G33">
+        <v>427.495</v>
+      </c>
+      <c r="H33">
+        <v>109.3250955</v>
+      </c>
+      <c r="I33">
         <v>10</v>
       </c>
-      <c r="D33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33">
-        <v>179</v>
-      </c>
-      <c r="G33">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H33">
-        <v>328.677753</v>
-      </c>
-      <c r="I33">
-        <v>9</v>
-      </c>
       <c r="J33">
-        <v>87.221436870000005</v>
+        <v>218.31</v>
       </c>
       <c r="K33">
-        <v>63.515759969999998</v>
+        <v>185.94640010000001</v>
       </c>
       <c r="L33">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="M33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N33">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O33" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="P33" t="s">
         <v>25</v>
       </c>
       <c r="Q33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R33">
-        <v>6.25E-2</v>
+        <v>0.1</v>
       </c>
       <c r="S33">
-        <v>179</v>
-      </c>
-      <c r="T33" t="s">
-        <v>22</v>
+        <v>101.2</v>
+      </c>
+      <c r="T33">
+        <v>22.519264400000001</v>
       </c>
       <c r="U33" t="s">
         <v>26</v>
       </c>
-      <c r="V33" t="s">
-        <v>22</v>
+      <c r="V33">
+        <v>60</v>
       </c>
       <c r="W33" t="s">
         <v>22</v>
       </c>
       <c r="X33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" t="s">
-        <v>22</v>
-      </c>
-      <c r="F34">
-        <v>150</v>
-      </c>
-      <c r="G34">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H34">
-        <v>328.677753</v>
-      </c>
-      <c r="I34">
-        <v>9</v>
-      </c>
-      <c r="J34">
-        <v>181.832157</v>
-      </c>
-      <c r="K34">
-        <v>47.298146269999997</v>
-      </c>
-      <c r="L34">
-        <v>9</v>
-      </c>
-      <c r="M34" t="s">
-        <v>37</v>
-      </c>
-      <c r="N34">
-        <v>21</v>
-      </c>
-      <c r="O34" t="s">
-        <v>33</v>
-      </c>
-      <c r="P34" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q34">
-        <v>2</v>
-      </c>
-      <c r="R34">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S34">
-        <v>150</v>
-      </c>
-      <c r="T34" t="s">
-        <v>22</v>
-      </c>
-      <c r="U34" t="s">
-        <v>26</v>
-      </c>
-      <c r="V34" t="s">
-        <v>22</v>
-      </c>
-      <c r="W34" t="s">
-        <v>22</v>
-      </c>
-      <c r="X34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35">
-        <v>179</v>
-      </c>
-      <c r="G35">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H35">
-        <v>328.677753</v>
-      </c>
-      <c r="I35">
-        <v>9</v>
-      </c>
-      <c r="J35">
-        <v>51.292534230000001</v>
-      </c>
-      <c r="K35">
-        <v>49.333246719999998</v>
-      </c>
-      <c r="L35">
-        <v>16</v>
-      </c>
-      <c r="M35" t="s">
-        <v>37</v>
-      </c>
-      <c r="N35">
-        <v>21</v>
-      </c>
-      <c r="O35" t="s">
-        <v>33</v>
-      </c>
-      <c r="P35" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q35">
-        <v>2</v>
-      </c>
-      <c r="R35">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S35">
-        <v>179</v>
-      </c>
-      <c r="T35" t="s">
-        <v>22</v>
-      </c>
-      <c r="U35" t="s">
-        <v>26</v>
-      </c>
-      <c r="V35" t="s">
-        <v>22</v>
-      </c>
-      <c r="W35" t="s">
-        <v>22</v>
-      </c>
-      <c r="X35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
         <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36">
-        <v>179</v>
-      </c>
-      <c r="G36">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H36">
-        <v>328.677753</v>
-      </c>
-      <c r="I36">
-        <v>9</v>
-      </c>
-      <c r="J36">
-        <v>67.347826119999993</v>
-      </c>
-      <c r="K36">
-        <v>69.933008979999997</v>
-      </c>
-      <c r="L36">
-        <v>16</v>
-      </c>
-      <c r="M36" t="s">
-        <v>37</v>
-      </c>
-      <c r="N36">
-        <v>21</v>
-      </c>
-      <c r="O36" t="s">
-        <v>33</v>
-      </c>
-      <c r="P36" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q36">
-        <v>2</v>
-      </c>
-      <c r="R36">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S36">
-        <v>179</v>
-      </c>
-      <c r="T36" t="s">
-        <v>22</v>
-      </c>
-      <c r="U36" t="s">
-        <v>26</v>
-      </c>
-      <c r="V36" t="s">
-        <v>22</v>
-      </c>
-      <c r="W36" t="s">
-        <v>22</v>
-      </c>
-      <c r="X36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37">
-        <v>179</v>
-      </c>
-      <c r="G37">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H37">
-        <v>328.677753</v>
-      </c>
-      <c r="I37">
-        <v>9</v>
-      </c>
-      <c r="J37">
-        <v>58.766026170000004</v>
-      </c>
-      <c r="K37">
-        <v>46.16436693</v>
-      </c>
-      <c r="L37">
-        <v>16</v>
-      </c>
-      <c r="M37" t="s">
-        <v>37</v>
-      </c>
-      <c r="N37">
-        <v>21</v>
-      </c>
-      <c r="O37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P37" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q37">
-        <v>2</v>
-      </c>
-      <c r="R37">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S37">
-        <v>179</v>
-      </c>
-      <c r="T37" t="s">
-        <v>22</v>
-      </c>
-      <c r="U37" t="s">
-        <v>26</v>
-      </c>
-      <c r="V37" t="s">
-        <v>22</v>
-      </c>
-      <c r="W37" t="s">
-        <v>22</v>
-      </c>
-      <c r="X37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F38">
-        <v>179</v>
-      </c>
-      <c r="G38">
-        <v>565.10414960000003</v>
-      </c>
-      <c r="H38">
-        <v>328.677753</v>
-      </c>
-      <c r="I38">
-        <v>9</v>
-      </c>
-      <c r="J38">
-        <v>68.78087386</v>
-      </c>
-      <c r="K38">
-        <v>65.25066726</v>
-      </c>
-      <c r="L38">
-        <v>16</v>
-      </c>
-      <c r="M38" t="s">
-        <v>37</v>
-      </c>
-      <c r="N38">
-        <v>21</v>
-      </c>
-      <c r="O38" t="s">
-        <v>33</v>
-      </c>
-      <c r="P38" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q38">
-        <v>2</v>
-      </c>
-      <c r="R38">
-        <v>6.25E-2</v>
-      </c>
-      <c r="S38">
-        <v>179</v>
-      </c>
-      <c r="T38" t="s">
-        <v>22</v>
-      </c>
-      <c r="U38" t="s">
-        <v>26</v>
-      </c>
-      <c r="V38" t="s">
-        <v>22</v>
-      </c>
-      <c r="W38" t="s">
-        <v>22</v>
-      </c>
-      <c r="X38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39">
-        <v>154.482125</v>
-      </c>
-      <c r="G39">
-        <v>333.47</v>
-      </c>
-      <c r="H39">
-        <v>40.73364703</v>
-      </c>
-      <c r="I39">
-        <v>4</v>
-      </c>
-      <c r="J39">
-        <v>135.80000000000001</v>
-      </c>
-      <c r="K39">
-        <v>20.751983039999999</v>
-      </c>
-      <c r="L39">
-        <v>4</v>
-      </c>
-      <c r="M39" t="s">
-        <v>37</v>
-      </c>
-      <c r="N39">
-        <v>23</v>
-      </c>
-      <c r="O39" t="s">
-        <v>24</v>
-      </c>
-      <c r="P39" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-      <c r="R39">
-        <v>0.16</v>
-      </c>
-      <c r="S39">
-        <v>154.482125</v>
-      </c>
-      <c r="T39" t="s">
-        <v>22</v>
-      </c>
-      <c r="U39" t="s">
-        <v>26</v>
-      </c>
-      <c r="V39" t="s">
-        <v>22</v>
-      </c>
-      <c r="W39" t="s">
-        <v>22</v>
-      </c>
-      <c r="X39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40">
-        <v>103.5835</v>
-      </c>
-      <c r="G40">
-        <v>327.54000000000002</v>
-      </c>
-      <c r="H40">
-        <v>54.037106700000002</v>
-      </c>
-      <c r="I40">
-        <v>4</v>
-      </c>
-      <c r="J40">
-        <v>211.78</v>
-      </c>
-      <c r="K40">
-        <v>18.6400617</v>
-      </c>
-      <c r="L40">
-        <v>4</v>
-      </c>
-      <c r="M40" t="s">
-        <v>37</v>
-      </c>
-      <c r="N40">
-        <v>22</v>
-      </c>
-      <c r="O40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P40" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-      <c r="R40">
-        <v>0.16</v>
-      </c>
-      <c r="S40">
-        <v>103.5835</v>
-      </c>
-      <c r="T40">
-        <v>24.059328000000001</v>
-      </c>
-      <c r="U40" t="s">
-        <v>26</v>
-      </c>
-      <c r="V40">
-        <v>60</v>
-      </c>
-      <c r="W40" t="s">
-        <v>92</v>
-      </c>
-      <c r="X40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="F41">
-        <v>10</v>
-      </c>
-      <c r="G41">
-        <v>113.9</v>
-      </c>
-      <c r="H41">
-        <v>29.4</v>
-      </c>
-      <c r="I41">
-        <v>5</v>
-      </c>
-      <c r="J41">
-        <v>105.3</v>
-      </c>
-      <c r="K41">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="L41">
-        <v>5</v>
-      </c>
-      <c r="M41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N41">
-        <v>30</v>
-      </c>
-      <c r="O41" t="s">
-        <v>24</v>
-      </c>
-      <c r="P41" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-      <c r="R41">
-        <v>0.5</v>
-      </c>
-      <c r="S41">
-        <v>10</v>
-      </c>
-      <c r="T41">
-        <v>2</v>
-      </c>
-      <c r="U41" t="s">
-        <v>38</v>
-      </c>
-      <c r="V41">
-        <v>45</v>
-      </c>
-      <c r="W41" t="s">
-        <v>22</v>
-      </c>
-      <c r="X41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42">
-        <v>117.38</v>
-      </c>
-      <c r="G42">
-        <v>256</v>
-      </c>
-      <c r="H42">
-        <v>26.8</v>
-      </c>
-      <c r="I42">
-        <v>4</v>
-      </c>
-      <c r="J42">
-        <v>183.8</v>
-      </c>
-      <c r="K42">
-        <v>5.8</v>
-      </c>
-      <c r="L42">
-        <v>4</v>
-      </c>
-      <c r="M42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N42">
-        <v>24</v>
-      </c>
-      <c r="O42" t="s">
-        <v>24</v>
-      </c>
-      <c r="P42" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-      <c r="R42">
-        <v>0.25</v>
-      </c>
-      <c r="S42">
-        <v>117.38</v>
-      </c>
-      <c r="T42" t="s">
-        <v>22</v>
-      </c>
-      <c r="U42" t="s">
-        <v>26</v>
-      </c>
-      <c r="V42">
-        <v>60</v>
-      </c>
-      <c r="W42" t="s">
-        <v>22</v>
-      </c>
-      <c r="X42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43">
-        <v>21</v>
-      </c>
-      <c r="F43">
-        <v>-9999</v>
-      </c>
-      <c r="G43">
-        <v>442.15679999999998</v>
-      </c>
-      <c r="H43" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43">
-        <v>3</v>
-      </c>
-      <c r="J43">
-        <v>236.7577</v>
-      </c>
-      <c r="K43" t="s">
-        <v>22</v>
-      </c>
-      <c r="L43">
-        <v>3</v>
-      </c>
-      <c r="N43">
-        <v>27</v>
-      </c>
-      <c r="O43" t="s">
-        <v>24</v>
-      </c>
-      <c r="P43" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-      <c r="R43">
-        <v>6.25</v>
-      </c>
-      <c r="S43" t="s">
-        <v>22</v>
-      </c>
-      <c r="T43">
-        <v>21</v>
-      </c>
-      <c r="U43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44">
-        <v>10</v>
-      </c>
-      <c r="F44">
-        <v>-9999</v>
-      </c>
-      <c r="G44">
-        <v>406.6035</v>
-      </c>
-      <c r="H44" t="s">
-        <v>22</v>
-      </c>
-      <c r="I44">
-        <v>3</v>
-      </c>
-      <c r="J44">
-        <v>303.1123</v>
-      </c>
-      <c r="K44" t="s">
-        <v>22</v>
-      </c>
-      <c r="L44">
-        <v>3</v>
-      </c>
-      <c r="N44">
-        <v>29</v>
-      </c>
-      <c r="O44" t="s">
-        <v>24</v>
-      </c>
-      <c r="P44" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-      <c r="R44">
-        <v>6.25</v>
-      </c>
-      <c r="S44">
-        <v>38.826592419999997</v>
-      </c>
-      <c r="T44">
-        <v>10</v>
-      </c>
-      <c r="U44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45">
-        <v>8</v>
-      </c>
-      <c r="D45" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45">
-        <v>6.3</v>
-      </c>
-      <c r="F45">
-        <v>30</v>
-      </c>
-      <c r="G45">
-        <v>378</v>
-      </c>
-      <c r="H45">
-        <v>19</v>
-      </c>
-      <c r="I45">
-        <v>18</v>
-      </c>
-      <c r="J45">
-        <v>282</v>
-      </c>
-      <c r="K45">
-        <v>17</v>
-      </c>
-      <c r="L45">
-        <v>18</v>
-      </c>
-      <c r="M45" t="s">
-        <v>23</v>
-      </c>
-      <c r="N45">
-        <v>33</v>
-      </c>
-      <c r="O45" t="s">
-        <v>24</v>
-      </c>
-      <c r="P45" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q45">
-        <v>1</v>
-      </c>
-      <c r="R45">
-        <v>1</v>
-      </c>
-      <c r="S45">
-        <v>30</v>
-      </c>
-      <c r="T45">
-        <v>6.3</v>
-      </c>
-      <c r="U45" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46">
-        <v>11</v>
-      </c>
-      <c r="D46" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46">
-        <v>101.2</v>
-      </c>
-      <c r="G46">
-        <v>427.495</v>
-      </c>
-      <c r="H46">
-        <v>109.3250955</v>
-      </c>
-      <c r="I46">
-        <v>10</v>
-      </c>
-      <c r="J46">
-        <v>218.31</v>
-      </c>
-      <c r="K46">
-        <v>185.94640010000001</v>
-      </c>
-      <c r="L46">
-        <v>45</v>
-      </c>
-      <c r="M46" t="s">
-        <v>37</v>
-      </c>
-      <c r="N46">
-        <v>25</v>
-      </c>
-      <c r="O46" t="s">
-        <v>24</v>
-      </c>
-      <c r="P46" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q46">
-        <v>1</v>
-      </c>
-      <c r="R46">
-        <v>0.1</v>
-      </c>
-      <c r="S46">
-        <v>101.2</v>
-      </c>
-      <c r="T46">
-        <v>22.519264400000001</v>
-      </c>
-      <c r="U46" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>